<commit_message>
Auto-committed on 2022/05/19 週四 16:27:12.46
</commit_message>
<xml_diff>
--- a/Program/Other/L9704_底稿_催收款明細表.xlsx
+++ b/Program/Other/L9704_底稿_催收款明細表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87DB1CA-D29A-4E16-96EF-813673EBE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5704248D-8093-4246-822A-FEE02D337A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>地區別</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,18 +91,12 @@
     <t>程式ID：</t>
   </si>
   <si>
-    <t>L9803</t>
-  </si>
-  <si>
     <t>新光人壽保險股份有限公司</t>
   </si>
   <si>
     <t>報　表：</t>
   </si>
   <si>
-    <t>LM008</t>
-  </si>
-  <si>
     <t>催收款明細表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,6 +106,22 @@
   </si>
   <si>
     <t>時　　間：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>L9</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>704</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -119,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +162,13 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -263,29 +280,32 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,7 +590,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="C4" sqref="C4:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -581,7 +601,7 @@
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -590,106 +610,106 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="13"/>
+      <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" s="7" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="13"/>
+      <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="8"/>
     </row>
-    <row r="3" spans="1:16" s="10" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:16" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:16" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="7" t="s">
+      <c r="H5" s="14"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="7" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="9"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="13"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -744,18 +764,18 @@
   </sheetData>
   <autoFilter ref="A6:P6" xr:uid="{D20383FD-DAB1-41F4-B39A-FE4EB10F9773}"/>
   <mergeCells count="12">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="O5:P5"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="C2:N2"/>
     <mergeCell ref="C3:N3"/>
     <mergeCell ref="C4:N4"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="O5:P5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>